<commit_message>
Completed GNAAS WEB APP DB
</commit_message>
<xml_diff>
--- a/static/excel_template/zone_details.xlsx
+++ b/static/excel_template/zone_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ernes\OneDrive\Desktop\GNAAS PROJECT\static\excel_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{206809F7-8DC4-4D3E-B6C0-63834052A855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93918DF-30C8-4E9E-B405-FAAE1538CA86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{54C6E879-B1F8-400C-9DA7-92CDF3CE3389}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>SCHOOL_HOSTING</t>
   </si>
@@ -65,25 +65,10 @@
     <t>COORDINATING_SECRETARY_CONTACT</t>
   </si>
   <si>
-    <t>Accra City Zone</t>
-  </si>
-  <si>
-    <t>UG</t>
-  </si>
-  <si>
-    <t>Kwabena Ampong</t>
-  </si>
-  <si>
-    <t>Kafui Sandrah</t>
-  </si>
-  <si>
-    <t>Samba Doris</t>
-  </si>
-  <si>
-    <t>Prince Owusu</t>
-  </si>
-  <si>
     <t>ZONE_NAME</t>
+  </si>
+  <si>
+    <t>ACADEMIC_YEAR</t>
   </si>
 </sst>
 </file>
@@ -475,87 +460,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17FA658C-323C-417B-AEBC-895D540E4261}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2">
-        <v>54234592</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2">
-        <v>20554925</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2">
-        <v>59542235</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2">
-        <v>25853217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>